<commit_message>
Fixed tests that modify templates data
</commit_message>
<xml_diff>
--- a/Examples/templates/externalWorkbook.xlsx
+++ b/Examples/templates/externalWorkbook.xlsx
@@ -1,121 +1,107 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<ssml:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ssml="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <ssml:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <ssml:workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <ssml:bookViews>
-    <ssml:workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
-  </ssml:bookViews>
-  <ssml:sheets>
-    <ssml:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </ssml:sheets>
-  <ssml:calcPr calcId="122211"/>
-</ssml:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC516EC1-3842-4097-B1E8-D0CDCA36227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="122211"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<ssml:sst xmlns:ssml="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <ssml:si>
-    <ssml:t xml:space="preserve"> </ssml:t>
-  </ssml:si>
-  <ssml:si>
-    <ssml:t>Sales</ssml:t>
-  </ssml:si>
-  <ssml:si>
-    <ssml:t>1st Qtr</ssml:t>
-  </ssml:si>
-  <ssml:si>
-    <ssml:t>2nd Qtr</ssml:t>
-  </ssml:si>
-  <ssml:si>
-    <ssml:t>3rd Qtr</ssml:t>
-  </ssml:si>
-  <ssml:si>
-    <ssml:t>4th Qtr</ssml:t>
-  </ssml:si>
-</ssml:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>1st Qtr</t>
+  </si>
+  <si>
+    <t>2nd Qtr</t>
+  </si>
+  <si>
+    <t>3rd Qtr</t>
+  </si>
+  <si>
+    <t>4th Qtr</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<ssml:styleSheet xmlns:ssml="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <ssml:fonts count="1">
-    <ssml:font>
-      <ssml:sz val="11"/>
-      <ssml:color theme="1"/>
-      <ssml:name val="Calibri"/>
-      <ssml:family val="2"/>
-      <ssml:charset val="204"/>
-      <ssml:scheme val="minor"/>
-    </ssml:font>
-  </ssml:fonts>
-  <ssml:fills count="2">
-    <ssml:fill>
-      <ssml:patternFill patternType="none"/>
-    </ssml:fill>
-    <ssml:fill>
-      <ssml:patternFill patternType="gray125"/>
-    </ssml:fill>
-  </ssml:fills>
-  <ssml:borders count="1">
-    <ssml:border>
-      <ssml:left/>
-      <ssml:right/>
-      <ssml:top/>
-      <ssml:bottom/>
-      <ssml:diagonal/>
-    </ssml:border>
-  </ssml:borders>
-  <ssml:cellStyleXfs count="1">
-    <ssml:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </ssml:cellStyleXfs>
-  <ssml:cellXfs count="2">
-    <ssml:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <ssml:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-  </ssml:cellXfs>
-  <ssml:cellStyles count="1">
-    <ssml:cellStyle name="Обычный" xfId="0" builtinId="0"/>
-  </ssml:cellStyles>
-  <ssml:dxfs count="1">
-    <ssml:dxf>
-      <ssml:border diagonalUp="0" diagonalDown="0">
-        <ssml:left style="thin">
-          <ssml:color indexed="12"/>
-        </ssml:left>
-        <ssml:right style="thin">
-          <ssml:color indexed="12"/>
-        </ssml:right>
-        <ssml:top style="thin">
-          <ssml:color indexed="12"/>
-        </ssml:top>
-        <ssml:bottom style="thin">
-          <ssml:color indexed="12"/>
-        </ssml:bottom>
-      </ssml:border>
-    </ssml:dxf>
-  </ssml:dxfs>
-  <ssml:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <ssml:extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-  </ssml:extLst>
-</ssml:styleSheet>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<ssml:table xmlns:ssml="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B5">
-  <ssml:tableColumns count="2">
-    <ssml:tableColumn id="1" name=" "/>
-    <ssml:tableColumn id="2" name="Sales"/>
-  </ssml:tableColumns>
-  <ssml:tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</ssml:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name=" "/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sales"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,9 +139,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +173,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +225,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -396,60 +418,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<ssml:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ssml="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <ssml:dimension ref="A1"/>
-  <ssml:sheetViews>
-    <ssml:sheetView tabSelected="1" workbookViewId="0">
-      <ssml:selection activeCell="A1"/>
-    </ssml:sheetView>
-  </ssml:sheetViews>
-  <ssml:sheetFormatPr defaultRowHeight="15"/>
-  <ssml:sheetData>
-    <ssml:row r="1">
-      <ssml:c r="A1" t="s">
-        <ssml:v>0</ssml:v>
-      </ssml:c>
-      <ssml:c r="B1" t="s">
-        <ssml:v>1</ssml:v>
-      </ssml:c>
-    </ssml:row>
-    <ssml:row r="2">
-      <ssml:c r="A2" t="s">
-        <ssml:v>2</ssml:v>
-      </ssml:c>
-      <ssml:c r="B2">
-        <ssml:v>100</ssml:v>
-      </ssml:c>
-    </ssml:row>
-    <ssml:row r="3">
-      <ssml:c r="A3" t="s">
-        <ssml:v>3</ssml:v>
-      </ssml:c>
-      <ssml:c r="B3">
-        <ssml:v>3.2</ssml:v>
-      </ssml:c>
-    </ssml:row>
-    <ssml:row r="4">
-      <ssml:c r="A4" t="s">
-        <ssml:v>4</ssml:v>
-      </ssml:c>
-      <ssml:c r="B4">
-        <ssml:v>1.4</ssml:v>
-      </ssml:c>
-    </ssml:row>
-    <ssml:row r="5">
-      <ssml:c r="A5" t="s">
-        <ssml:v>5</ssml:v>
-      </ssml:c>
-      <ssml:c r="B5">
-        <ssml:v>1.2</ssml:v>
-      </ssml:c>
-    </ssml:row>
-  </ssml:sheetData>
-  <ssml:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ssml:pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-  <ssml:tableParts>
-    <ssml:tablePart r:id="rId2"/>
-  </ssml:tableParts>
-</ssml:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>